<commit_message>
ben/alpha-06: remove github plugin folder
</commit_message>
<xml_diff>
--- a/Assets/Plans/Cards_and_Classes.xlsx
+++ b/Assets/Plans/Cards_and_Classes.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Card Game 2020\Assets\Plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Unity\Unity-Card-Game-2020\Assets\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19328DA-40BC-401E-82DD-B4C7D8208F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
   <si>
     <t>Card Name</t>
   </si>
@@ -148,9 +147,6 @@
     <t>Gain 2 will</t>
   </si>
   <si>
-    <t>1 enemy gets -5 damage for the turn</t>
-  </si>
-  <si>
     <t>Whirling Bones</t>
   </si>
   <si>
@@ -307,12 +303,6 @@
     <t>Cyclops</t>
   </si>
   <si>
-    <t>Summon 1 skeleton (10 health, 5 dmg/turn)</t>
-  </si>
-  <si>
-    <t>Summon 1 spirit (can't be attacked, enemies lose x damage equal to spirits in play)</t>
-  </si>
-  <si>
     <t>Unc/Rare</t>
   </si>
   <si>
@@ -328,9 +318,6 @@
     <t>Increase damage reduction applied by spirits by 1</t>
   </si>
   <si>
-    <t>Summon 1 zombie (1 health, attack for 1 infection, on death apply 1 infection to the enemy)</t>
-  </si>
-  <si>
     <t>2 infection for each zombie to target</t>
   </si>
   <si>
@@ -464,12 +451,42 @@
   </si>
   <si>
     <t>Increase summon slots by 2, draw 2 cards</t>
+  </si>
+  <si>
+    <t>Key Draft Strats:</t>
+  </si>
+  <si>
+    <t>Spirit Combo</t>
+  </si>
+  <si>
+    <t>Zombie DOT</t>
+  </si>
+  <si>
+    <t>Summon Value</t>
+  </si>
+  <si>
+    <t>Mummy Damage</t>
+  </si>
+  <si>
+    <t>Sacrifice</t>
+  </si>
+  <si>
+    <t>Summon 1 skeleton (20 health, 3x2 attack)</t>
+  </si>
+  <si>
+    <t>Summon 1 spirit (can't be attacked, once per turn random card in hand gets -5 cost for battle)</t>
+  </si>
+  <si>
+    <t>Summon 1 zombie (1 health, 1 attack, 1 infection, attacks do not trample over)</t>
+  </si>
+  <si>
+    <t>1 enemy gets -5 attack for the turn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -789,11 +806,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,13 +830,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -862,25 +879,25 @@
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -903,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -923,7 +940,7 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -943,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>93</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -954,7 +971,7 @@
         <v>24</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
         <v>31</v>
@@ -963,7 +980,7 @@
         <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -991,7 +1008,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,19 +1016,19 @@
         <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D17">
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1019,106 +1036,121 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D20">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>143</v>
+      </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D22">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>144</v>
+      </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D23">
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>145</v>
+      </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H24" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>146</v>
+      </c>
       <c r="C25" t="s">
         <v>15</v>
       </c>
@@ -1126,42 +1158,45 @@
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>147</v>
+      </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F26" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D27">
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -1170,7 +1205,7 @@
         <v>6</v>
       </c>
       <c r="H33" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -1181,7 +1216,7 @@
         <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1192,7 +1227,7 @@
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -1203,7 +1238,7 @@
         <v>5</v>
       </c>
       <c r="H36" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -1214,29 +1249,29 @@
         <v>5</v>
       </c>
       <c r="H37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -1247,10 +1282,10 @@
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H44" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -1258,15 +1293,15 @@
         <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C54" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H54" t="s">
         <v>10</v>
@@ -1274,24 +1309,24 @@
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D55">
         <v>10</v>
       </c>
       <c r="H55" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D56">
         <v>3</v>
       </c>
       <c r="H56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -1301,7 +1336,7 @@
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -1316,35 +1351,35 @@
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H65" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H66" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D71">
         <v>2</v>
       </c>
       <c r="F71" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H71" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
@@ -1352,13 +1387,13 @@
         <v>2</v>
       </c>
       <c r="F72" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G72">
         <v>1</v>
       </c>
       <c r="H72" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
@@ -1366,10 +1401,10 @@
         <v>5</v>
       </c>
       <c r="F73" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
@@ -1377,7 +1412,7 @@
         <v>4</v>
       </c>
       <c r="H74" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1387,7 +1422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1404,145 +1439,145 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
         <v>70</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ben/alpha-13: change card template, add elements, add mummies, add starter deck
</commit_message>
<xml_diff>
--- a/Assets/Plans/Cards_and_Classes.xlsx
+++ b/Assets/Plans/Cards_and_Classes.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Characters" sheetId="1" r:id="rId1"/>
     <sheet name="Defect reference" sheetId="3" r:id="rId2"/>
     <sheet name="Enemies" sheetId="2" r:id="rId3"/>
+    <sheet name="Artifacts" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,29 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="348">
   <si>
     <t>Card Name</t>
   </si>
   <si>
-    <t>Earth: E</t>
-  </si>
-  <si>
-    <t>Air: A</t>
-  </si>
-  <si>
-    <t>Fire: F</t>
-  </si>
-  <si>
-    <t>Water: W</t>
-  </si>
-  <si>
-    <t>Life: L</t>
-  </si>
-  <si>
-    <t>Death: D</t>
-  </si>
-  <si>
     <t>Grasping Hands</t>
   </si>
   <si>
@@ -106,9 +89,6 @@
     <t>Quick Study</t>
   </si>
   <si>
-    <t>Artifice: R</t>
-  </si>
-  <si>
     <t>DR</t>
   </si>
   <si>
@@ -331,9 +311,6 @@
     <t>summon 1 zombie, 1 skeleton, 1 spirit</t>
   </si>
   <si>
-    <t>Meat Shields</t>
-  </si>
-  <si>
     <t>summon 2 zombies</t>
   </si>
   <si>
@@ -475,9 +452,6 @@
     <t>summon 2 mummies</t>
   </si>
   <si>
-    <t>Invoke the Curse</t>
-  </si>
-  <si>
     <t>Target zombie performs 2 attacks</t>
   </si>
   <si>
@@ -680,6 +654,423 @@
   </si>
   <si>
     <t>Move a summon to the back, draw a card</t>
+  </si>
+  <si>
+    <t>sacrifice a summon: random card in hand is free for the remainder of the turn</t>
+  </si>
+  <si>
+    <t>Primary summon mechanics:</t>
+  </si>
+  <si>
+    <t>Curse</t>
+  </si>
+  <si>
+    <t>Undying</t>
+  </si>
+  <si>
+    <t>Infector</t>
+  </si>
+  <si>
+    <t>On attack or death, apply 1 Infection to defender/killer (DOT after combat)</t>
+  </si>
+  <si>
+    <t>Whenever curse is applied, deal damage equal to curse value to random enemy</t>
+  </si>
+  <si>
+    <t>Thoughts on the Necromancer:</t>
+  </si>
+  <si>
+    <t>Generally, should not be hit directly by enemy attacks. Summons primarily soak up damage.</t>
+  </si>
+  <si>
+    <t>In doing so, the "cost" of being safe is that summons still require life to summon.</t>
+  </si>
+  <si>
+    <t>The difficulty aspect of the necromancer is maintaining damage velocity while its summons are being killed every turn.</t>
+  </si>
+  <si>
+    <t>Maybe summons should attack before enemies? Concerns this may make summons too strong</t>
+  </si>
+  <si>
+    <t>Initial difficulty ramping thoughts:</t>
+  </si>
+  <si>
+    <t>Difficulty should probably ramp up quickly though</t>
+  </si>
+  <si>
+    <t>10 "Floors" per act - about 3-5 low level fights, 1-3 "elite" enemy fights, 1 final boss</t>
+  </si>
+  <si>
+    <t>The primary focus of the non-combat encounters is "cards are a currency"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power spike moments in the runs are shops. </t>
+  </si>
+  <si>
+    <t>Should only be 1-2 rares available in shops on average. ~25% of the time: no rares, %50 of the time: 1 rare, %25 of the time: 2 rares</t>
+  </si>
+  <si>
+    <t>To prevent the player from downsizing their deck immediately but not directly "gate" the player from trading how they want, rares will be infrequent in shops</t>
+  </si>
+  <si>
+    <t>Artifacts will also be available for purchase in the shop.</t>
+  </si>
+  <si>
+    <t>Non-combat</t>
+  </si>
+  <si>
+    <t>Question: should newly acquired cards be allowed to be traded back? E.G. pick up uncommon, then exchange for rare -&gt; essentially trading common at uncommon value</t>
+  </si>
+  <si>
+    <t>Common artifacts are 1:1 for any card. Uncommon artifacts require 2:1 (rare/uncommon count for 2). Rare artifacts are 3:1 (uncommon is 2, rare is 3).</t>
+  </si>
+  <si>
+    <t>Total number of cards seen in shop will be 5-10, final number not totally decided.</t>
+  </si>
+  <si>
+    <t>Get an extra card shown in rewards if deck over a certain size? (e.g. from 3 -&gt; 4 cards shown)</t>
+  </si>
+  <si>
+    <t>Cards: Commons are not in shops. Uncommons can be acquired by trading in commons 1:1. Rares are acquired by trading in commons 3:1 (uncommons count as 2).</t>
+  </si>
+  <si>
+    <t>Similar rare drop rates</t>
+  </si>
+  <si>
+    <t>The last primary function of the shop is healing. Trade 1 card in to heal. Based on deck size and card traded in, will is healed a certain amount</t>
+  </si>
+  <si>
+    <t>Gain 1 will for deck size/x + y*card rarity … General idea of the healing formula</t>
+  </si>
+  <si>
+    <t>x=5, y=2. With a deck size of 15, trade in rare card for 9 will. Trade in uncommon for 7 will. Trade in common for 5 will.</t>
+  </si>
+  <si>
+    <t>Possibly considering making artifacts more "expensive". Depends on what the total number of artifacts expected to receive in a run is</t>
+  </si>
+  <si>
+    <t>There could be a gate/incentive against making deck size small. Player takes damage on deck cycle (don't like this), Rewards related on deck-size (much better)</t>
+  </si>
+  <si>
+    <t>On will -&gt; life conversion: the amount of life received when trading in 1 will is a set value called "Life Ratio". It can be increased temporarily or permanently</t>
+  </si>
+  <si>
+    <t>The amount of life available to be spent per turn is equal to the player's life ratio.</t>
+  </si>
+  <si>
+    <t>Going off the baseline hero: Max/Starting Will: 20, Starting Life Ratio: 20</t>
+  </si>
+  <si>
+    <t>Initial Act 1 enemies probably shouldn't be able to deal much/any damage to a character (directly)</t>
+  </si>
+  <si>
+    <t>With 3 Acts, assuming primarily common card rewards with a sprinkling of uncommon, player will get about ~30 new card drafts before finale</t>
+  </si>
+  <si>
+    <t>Elite enemies will drop additional rewards in some way - perhaps an additional card pick, an artifact drop/draft, permanent upgrade to life ratio?</t>
+  </si>
+  <si>
+    <t>Some artifacts will provide values/effects regardless of affinities</t>
+  </si>
+  <si>
+    <t>The more powerful/splashy artifacts should probably rely on affinities though</t>
+  </si>
+  <si>
+    <t>Artifacts</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Required affinities</t>
+  </si>
+  <si>
+    <t>Draw a card</t>
+  </si>
+  <si>
+    <t>When will is below half, increase life ratio by 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whenever a card is played, </t>
+  </si>
+  <si>
+    <t>Zombies are summoned with an additional 2 infect</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Unique Character</t>
+  </si>
+  <si>
+    <t>Weaken all enemy attacks this turn by 1</t>
+  </si>
+  <si>
+    <t>Summon a Zombie</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>Necromancer</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Gain 3 life</t>
+  </si>
+  <si>
+    <t>Uncommon</t>
+  </si>
+  <si>
+    <t>Increase life ratio by 2 until end of combat</t>
+  </si>
+  <si>
+    <t>+1 Draw per turn (and immediately draw a card) until end of combat</t>
+  </si>
+  <si>
+    <t>Gain 5 curse (on the player character)</t>
+  </si>
+  <si>
+    <t>So if an affinity requires WWW and only WW is gained on a turn,</t>
+  </si>
+  <si>
+    <t>That WW persists on the artifact until a third W is gained or combat ends</t>
+  </si>
+  <si>
+    <t>Gain an attack this turn (on the player character)</t>
+  </si>
+  <si>
+    <t>Gain an attack until end of combat (on the player character)</t>
+  </si>
+  <si>
+    <t>Gain 2 elements of your choice (does not trigger this effect)</t>
+  </si>
+  <si>
+    <t>Elements contributed to affinities are not lost between turns.</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Reserve means the card is not disarded at the end of the turn</t>
+  </si>
+  <si>
+    <t>Apply "Reserve" to a card in hand until the end of the turn</t>
+  </si>
+  <si>
+    <t>Kill an enemy</t>
+  </si>
+  <si>
+    <t>3A,3E,3F,3W,3L,3D,3R</t>
+  </si>
+  <si>
+    <t>3W</t>
+  </si>
+  <si>
+    <t>2W</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>2E</t>
+  </si>
+  <si>
+    <t>2F</t>
+  </si>
+  <si>
+    <t>2L</t>
+  </si>
+  <si>
+    <t>2R</t>
+  </si>
+  <si>
+    <t>Gain 1 Will</t>
+  </si>
+  <si>
+    <t>4L</t>
+  </si>
+  <si>
+    <t>Draw a card, reduce its cost by 3</t>
+  </si>
+  <si>
+    <t>2W,2R</t>
+  </si>
+  <si>
+    <t>4W</t>
+  </si>
+  <si>
+    <t>Draw 3 cards, put 2 cards in hand back on top of the deck</t>
+  </si>
+  <si>
+    <t>Brainstorm</t>
+  </si>
+  <si>
+    <t>Card is removed from the game for the rest of combat (returns to the deck after)</t>
+  </si>
+  <si>
+    <t>May exile a card in discard</t>
+  </si>
+  <si>
+    <t>May exile a card in discard, a card in hand, a card in deck</t>
+  </si>
+  <si>
+    <t>4D</t>
+  </si>
+  <si>
+    <t>*Highly subject to change</t>
+  </si>
+  <si>
+    <t>Elements and general focuses</t>
+  </si>
+  <si>
+    <t>Permanently add 1 more of an existing element to a card in hand</t>
+  </si>
+  <si>
+    <t>5E</t>
+  </si>
+  <si>
+    <t>Fire (F): Damage to enemies, strength buffs to player</t>
+  </si>
+  <si>
+    <t>Water (W): Card draw/selection</t>
+  </si>
+  <si>
+    <t>Life (L): Lifegain, life ratio, etc.</t>
+  </si>
+  <si>
+    <t>Artifice (R): Misc. card buffs</t>
+  </si>
+  <si>
+    <t>Repeat the next card play</t>
+  </si>
+  <si>
+    <t>Repeat the next artifact trigger</t>
+  </si>
+  <si>
+    <t>Remove all debuffs and negative statuses</t>
+  </si>
+  <si>
+    <t>3R</t>
+  </si>
+  <si>
+    <t>May apply "Reserve" to a card in your hand permanently</t>
+  </si>
+  <si>
+    <t>2F,2W</t>
+  </si>
+  <si>
+    <t>3E</t>
+  </si>
+  <si>
+    <t>2A,2L</t>
+  </si>
+  <si>
+    <t>2D,2R</t>
+  </si>
+  <si>
+    <t>Gain 1 of each element</t>
+  </si>
+  <si>
+    <t>Random card in hand costs 0 until end of battle</t>
+  </si>
+  <si>
+    <t>Random card in hand has double element until end of battle</t>
+  </si>
+  <si>
+    <t>At the end of combat, gain 1 will</t>
+  </si>
+  <si>
+    <t>Deal 2 damage to each enemy</t>
+  </si>
+  <si>
+    <t>Repeat the next card played</t>
+  </si>
+  <si>
+    <t>Death (D): Exiling cards, curse, discard pile</t>
+  </si>
+  <si>
+    <t>Return a card from discard to hand</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>Trigger another artifact of your choice (resets affinities)</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Should loosely follow a 3:1 ratio of mono:2+ element artifacts</t>
+  </si>
+  <si>
+    <t>Triggered or Passive</t>
+  </si>
+  <si>
+    <t>Triggered</t>
+  </si>
+  <si>
+    <t>Passive</t>
+  </si>
+  <si>
+    <t>6L</t>
+  </si>
+  <si>
+    <t>Reduce merchant card trade-in cost by 1</t>
+  </si>
+  <si>
+    <t>Reduce merchant artifact trade-in cost by 1</t>
+  </si>
+  <si>
+    <t>When you exile a card, gain 5 life</t>
+  </si>
+  <si>
+    <t>L,D</t>
+  </si>
+  <si>
+    <t>Increase life ratio by 3</t>
+  </si>
+  <si>
+    <t>Enemies do not attack on the first turn of battle</t>
+  </si>
+  <si>
+    <t>Add copy of a card in discard to your hand (stays until end of battle)</t>
+  </si>
+  <si>
+    <t>Deal damage to a random enemy equal to the number of cards in discard</t>
+  </si>
+  <si>
+    <t>F,D</t>
+  </si>
+  <si>
+    <t>Earth (E): Reduce incoming damage from enemies (defense/blocking)</t>
+  </si>
+  <si>
+    <t>Air (A): Add/change elements, affinities</t>
+  </si>
+  <si>
+    <t>Random enemy loses an attack this turn</t>
+  </si>
+  <si>
+    <t>Raise Dead</t>
+  </si>
+  <si>
+    <t>Invoked Curse</t>
   </si>
 </sst>
 </file>
@@ -723,9 +1114,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,481 +1405,478 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="84.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="99.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="I11" t="s">
+        <v>216</v>
+      </c>
+      <c r="K11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="K12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="K13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="K14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>347</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>346</v>
       </c>
       <c r="D18">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D19">
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="I19" t="s">
+        <v>210</v>
+      </c>
+      <c r="J19" t="s">
+        <v>213</v>
+      </c>
+      <c r="K19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D20">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="J20" t="s">
+        <v>211</v>
+      </c>
+      <c r="K20" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="J21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="H22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D23">
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H23" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D26">
         <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D27">
         <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F29" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D30">
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H31" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>6</v>
       </c>
       <c r="H33" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D36">
         <v>5</v>
       </c>
       <c r="H36" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H38" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
@@ -1488,12 +1884,12 @@
         <v>6</v>
       </c>
       <c r="H39" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
@@ -1501,7 +1897,7 @@
         <v>4</v>
       </c>
       <c r="H41" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
@@ -1509,218 +1905,189 @@
         <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D43">
         <v>10</v>
       </c>
       <c r="H43" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="H46" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H47" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D48">
         <v>8</v>
       </c>
       <c r="H48" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H49" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" t="s">
-        <v>90</v>
-      </c>
-      <c r="D51">
-        <v>4</v>
-      </c>
-      <c r="H51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52">
-        <v>10</v>
-      </c>
-      <c r="H52" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="H53" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>211</v>
-      </c>
-      <c r="D54">
-        <v>5</v>
-      </c>
-      <c r="H54" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
+      </c>
+      <c r="C56" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57">
+        <v>10</v>
+      </c>
       <c r="H57" t="s">
-        <v>145</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>0</v>
+      </c>
       <c r="H58" t="s">
-        <v>146</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
       <c r="H59" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D60">
-        <v>5</v>
-      </c>
-      <c r="H60" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="H61" t="s">
-        <v>208</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H62" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B63" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
-      </c>
-      <c r="F63" t="s">
-        <v>93</v>
-      </c>
       <c r="H63" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D64">
-        <v>2</v>
-      </c>
-      <c r="F64" t="s">
-        <v>93</v>
-      </c>
-      <c r="G64">
-        <v>1</v>
-      </c>
       <c r="H64" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D65">
         <v>5</v>
       </c>
-      <c r="F65" t="s">
-        <v>93</v>
-      </c>
       <c r="H65" t="s">
-        <v>128</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D66">
-        <v>4</v>
-      </c>
       <c r="H66" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H67" t="s">
-        <v>157</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B68" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="F68" t="s">
+        <v>86</v>
+      </c>
       <c r="H68" t="s">
-        <v>215</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="F69" t="s">
+        <v>86</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B70" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="D70">
         <v>5</v>
       </c>
+      <c r="F70" t="s">
+        <v>86</v>
+      </c>
       <c r="H70" t="s">
-        <v>216</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.3">
@@ -1728,54 +2095,88 @@
         <v>4</v>
       </c>
       <c r="H71" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H72" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C73" t="s">
-        <v>95</v>
-      </c>
-      <c r="D73">
+      <c r="H73" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D75">
         <v>5</v>
       </c>
-      <c r="H73" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H74" t="s">
+      <c r="H75" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>4</v>
+      </c>
+      <c r="H76" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H77" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78">
+        <v>5</v>
+      </c>
+      <c r="H78" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H79" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>10</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D75">
-        <v>10</v>
-      </c>
-      <c r="G75">
-        <v>1</v>
-      </c>
-      <c r="H75" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H76" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H81" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H82" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1788,20 +2189,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B1">
         <v>75</v>
@@ -1809,194 +2210,194 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2006,161 +2407,978 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
         <v>61</v>
       </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" t="s">
-        <v>76</v>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>229</v>
+      </c>
+      <c r="H23" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L86"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="60.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="2"/>
+    <col min="9" max="9" width="64.6640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E12" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D14" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D15" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D18" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D19" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D28" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E30" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E31" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E32" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="E33" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="E34" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="E36" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D38" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H39" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H40" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H41" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H42" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H44" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D48" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D49" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C50" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E53" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E54" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D55" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D56" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D57" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D58" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D59" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D61" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D62" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D63" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D64" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="68" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D68" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="71" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D71" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="72" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D72" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D73" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="76" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D76" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="77" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D77" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="78" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D78" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="79" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D79" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D82" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D83" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D84" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D85" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D86" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>